<commit_message>
Creating appropriate metadata files for data analysis
</commit_message>
<xml_diff>
--- a/Metadata Pan et al.xlsx
+++ b/Metadata Pan et al.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/berube_cardiff_ac_uk/Documents/Desktop/BI3008 2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/sullivan-al-kadhomiyj_cardiff_ac_uk/Documents/University/Masters/Big Data Biology/Modules/BIT103. Case Study/DATA/Case-Study_R-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{383FF813-71B4-47E5-BE3A-A1D55F56CB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DB46E52-2017-4E1C-A10D-3436792A004C}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{383FF813-71B4-47E5-BE3A-A1D55F56CB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5098F08-DD96-4C3A-8E09-1E06FE41275A}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="-120" windowWidth="27405" windowHeight="16440" xr2:uid="{D75F9A16-EBC4-4A40-B240-63730CF1E1F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D75F9A16-EBC4-4A40-B240-63730CF1E1F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>gender</t>
   </si>
@@ -135,6 +135,72 @@
   </si>
   <si>
     <t>201705CD0010</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>Sample Number</t>
   </si>
 </sst>
 </file>
@@ -147,7 +213,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +227,12 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,12 +242,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -184,28 +271,28 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -226,9 +313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -266,7 +353,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -372,7 +459,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -514,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -522,712 +609,767 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193912E2-BAE7-4241-921F-914B667C9C8A}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E2" s="5">
         <v>26</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>173</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>67</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>21.718066089745729</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>77.900000000000006</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>72.625698324022352</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>81.52</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E3" s="5">
         <v>24</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>168</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>60</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>21.513858510523864</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>101.3</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="6">
         <v>98.826979472140764</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>85.11</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5">
+      <c r="E4" s="5">
         <v>29</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>157</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>51</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>21.907582457706194</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>90.8</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>85.7638888888889</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>82.11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5">
+      <c r="E5" s="5">
         <v>23</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>150</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>50</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>20.811654526534856</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>104.4</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>107.03703703703704</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>89.02</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>26</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>160</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>52</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>19.531249999999996</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>86.7</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="6">
         <v>101.80180180180179</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>77.86</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E7" s="5">
         <v>22</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>178</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>83</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>25.880570635020831</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>107.7</v>
       </c>
-      <c r="I7" s="6">
+      <c r="J7" s="6">
         <v>77.524429967426713</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>79.81</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5">
+      <c r="E8" s="5">
         <v>29</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>167</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>65</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>22.589551436050055</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>110.4</v>
       </c>
-      <c r="I8" s="6">
+      <c r="J8" s="6">
         <v>105.71428571428572</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>81.540000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5">
+      <c r="E9" s="5">
         <v>33</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>160</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>58</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>22.656249999999996</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>105.6</v>
       </c>
-      <c r="I9" s="6">
+      <c r="J9" s="6">
         <v>102.91545189504372</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>83.11</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="5">
+      <c r="E10" s="5">
         <v>27</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>175</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>79</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>25.826446280991735</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>93.8</v>
       </c>
-      <c r="I10" s="6">
+      <c r="J10" s="6">
         <v>90.117647058823536</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>81.06</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="5">
+      <c r="E11" s="5">
         <v>38</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <v>167</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G11" s="5">
         <v>67</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>24.023808670084982</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>103.2</v>
       </c>
-      <c r="I11" s="6">
+      <c r="J11" s="6">
         <v>88.300835654596099</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>71.48</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J12" s="6"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="5">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8">
+        <v>163</v>
+      </c>
+      <c r="G13" s="8">
+        <v>52</v>
+      </c>
+      <c r="H13" s="3">
+        <v>19.571681282697881</v>
+      </c>
+      <c r="I13" s="1">
+        <v>113.8</v>
+      </c>
+      <c r="J13" s="1">
+        <v>108.7</v>
+      </c>
+      <c r="K13" s="1">
+        <v>96.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="5">
-        <v>22</v>
-      </c>
-      <c r="E14" s="8">
-        <v>163</v>
+      <c r="E14" s="5">
+        <v>28</v>
       </c>
       <c r="F14" s="8">
+        <v>169</v>
+      </c>
+      <c r="G14" s="8">
         <v>52</v>
       </c>
-      <c r="G14" s="3">
-        <v>19.571681282697881</v>
-      </c>
-      <c r="H14" s="1">
-        <v>113.8</v>
+      <c r="H14" s="3">
+        <v>18.381709323903227</v>
       </c>
       <c r="I14" s="1">
-        <v>108.7</v>
+        <v>106.6</v>
       </c>
       <c r="J14" s="1">
-        <v>96.42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>81.7</v>
+      </c>
+      <c r="K14" s="1">
+        <v>77.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5">
+        <v>25</v>
+      </c>
+      <c r="F15" s="8">
+        <v>168</v>
+      </c>
+      <c r="G15" s="8">
+        <v>50</v>
+      </c>
+      <c r="H15" s="3">
+        <v>17.006802721088437</v>
+      </c>
+      <c r="I15" s="1">
+        <v>105.3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>91.1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>87.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="5">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="F16" s="8">
+        <v>160</v>
+      </c>
+      <c r="G16" s="8">
+        <v>50</v>
+      </c>
+      <c r="H16" s="3">
+        <v>19.531249999999996</v>
+      </c>
+      <c r="I16" s="1">
+        <v>116.8</v>
+      </c>
+      <c r="J16" s="1">
+        <v>103.9</v>
+      </c>
+      <c r="K16" s="1">
+        <v>88.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="5">
+      <c r="E17" s="5">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8">
+        <v>160</v>
+      </c>
+      <c r="G17" s="8">
+        <v>55</v>
+      </c>
+      <c r="H17" s="3">
+        <v>21.75546853368142</v>
+      </c>
+      <c r="I17" s="1">
+        <v>89.3</v>
+      </c>
+      <c r="J17" s="1">
+        <v>89.2</v>
+      </c>
+      <c r="K17" s="1">
+        <v>99.27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="8">
-        <v>169</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="B18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="5">
+        <v>26</v>
+      </c>
+      <c r="F18" s="8">
+        <v>170</v>
+      </c>
+      <c r="G18" s="8">
+        <v>53</v>
+      </c>
+      <c r="H18" s="3">
+        <v>18.339100346020764</v>
+      </c>
+      <c r="I18" s="1">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="J18" s="1">
+        <v>80.7</v>
+      </c>
+      <c r="K18" s="1">
+        <v>97.58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="5">
+        <v>28</v>
+      </c>
+      <c r="F19" s="8">
+        <v>175</v>
+      </c>
+      <c r="G19" s="8">
+        <v>90</v>
+      </c>
+      <c r="H19" s="3">
+        <v>29.387755102040817</v>
+      </c>
+      <c r="I19" s="1">
+        <v>96.7</v>
+      </c>
+      <c r="J19" s="1">
+        <v>78</v>
+      </c>
+      <c r="K19" s="1">
+        <v>77.11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="5">
+        <v>25</v>
+      </c>
+      <c r="F20" s="8">
+        <v>178</v>
+      </c>
+      <c r="G20" s="8">
+        <v>100</v>
+      </c>
+      <c r="H20" s="3">
+        <v>31.561671506122963</v>
+      </c>
+      <c r="I20" s="1">
+        <v>100.5</v>
+      </c>
+      <c r="J20" s="1">
+        <v>103.3</v>
+      </c>
+      <c r="K20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="3">
-        <v>18.381709323903227</v>
-      </c>
-      <c r="H15" s="1">
-        <v>106.6</v>
-      </c>
-      <c r="I15" s="1">
-        <v>81.7</v>
-      </c>
-      <c r="J15" s="1">
-        <v>77.13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="5">
-        <v>25</v>
-      </c>
-      <c r="E16" s="8">
-        <v>168</v>
-      </c>
-      <c r="F16" s="8">
-        <v>50</v>
-      </c>
-      <c r="G16" s="3">
-        <v>17.006802721088437</v>
-      </c>
-      <c r="H16" s="1">
-        <v>105.3</v>
-      </c>
-      <c r="I16" s="1">
-        <v>91.1</v>
-      </c>
-      <c r="J16" s="1">
-        <v>87.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="E21" s="5">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8">
+        <v>173</v>
+      </c>
+      <c r="G21" s="8">
+        <v>81</v>
+      </c>
+      <c r="H21" s="3">
+        <v>27.064051588760066</v>
+      </c>
+      <c r="I21" s="1">
+        <v>91.9</v>
+      </c>
+      <c r="J21" s="1">
+        <v>94.4</v>
+      </c>
+      <c r="K21" s="1">
+        <v>96.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="5">
-        <v>24</v>
-      </c>
-      <c r="E17" s="8">
-        <v>160</v>
-      </c>
-      <c r="F17" s="8">
-        <v>50</v>
-      </c>
-      <c r="G17" s="3">
-        <v>19.531249999999996</v>
-      </c>
-      <c r="H17" s="1">
-        <v>116.8</v>
-      </c>
-      <c r="I17" s="1">
-        <v>103.9</v>
-      </c>
-      <c r="J17" s="1">
-        <v>88.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="5">
-        <v>25</v>
-      </c>
-      <c r="E18" s="8">
-        <v>160</v>
-      </c>
-      <c r="F18" s="8">
-        <v>55</v>
-      </c>
-      <c r="G18" s="3">
-        <v>21.75546853368142</v>
-      </c>
-      <c r="H18" s="1">
-        <v>89.3</v>
-      </c>
-      <c r="I18" s="1">
-        <v>89.2</v>
-      </c>
-      <c r="J18" s="1">
-        <v>99.27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="5">
-        <v>26</v>
-      </c>
-      <c r="E19" s="8">
-        <v>170</v>
-      </c>
-      <c r="F19" s="8">
-        <v>53</v>
-      </c>
-      <c r="G19" s="3">
-        <v>18.339100346020764</v>
-      </c>
-      <c r="H19" s="1">
-        <v>78.599999999999994</v>
-      </c>
-      <c r="I19" s="1">
-        <v>80.7</v>
-      </c>
-      <c r="J19" s="1">
-        <v>97.58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7" t="s">
+      <c r="E22" s="5">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="5">
-        <v>28</v>
-      </c>
-      <c r="E20" s="8">
-        <v>175</v>
-      </c>
-      <c r="F20" s="8">
-        <v>90</v>
-      </c>
-      <c r="G20" s="3">
-        <v>29.387755102040817</v>
-      </c>
-      <c r="H20" s="1">
-        <v>96.7</v>
-      </c>
-      <c r="I20" s="1">
-        <v>78</v>
-      </c>
-      <c r="J20" s="1">
-        <v>77.11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="5">
-        <v>25</v>
-      </c>
-      <c r="E21" s="8">
-        <v>178</v>
-      </c>
-      <c r="F21" s="8">
-        <v>100</v>
-      </c>
-      <c r="G21" s="3">
-        <v>31.561671506122963</v>
-      </c>
-      <c r="H21" s="1">
-        <v>100.5</v>
-      </c>
-      <c r="I21" s="1">
-        <v>103.3</v>
-      </c>
-      <c r="J21" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="5">
-        <v>30</v>
-      </c>
-      <c r="E22" s="8">
-        <v>173</v>
-      </c>
       <c r="F22" s="8">
-        <v>81</v>
-      </c>
-      <c r="G22" s="3">
-        <v>27.064051588760066</v>
-      </c>
-      <c r="H22" s="1">
-        <v>91.9</v>
+        <v>183</v>
+      </c>
+      <c r="G22" s="8">
+        <v>80</v>
+      </c>
+      <c r="H22" s="3">
+        <v>23.888440980620498</v>
       </c>
       <c r="I22" s="1">
-        <v>94.4</v>
+        <v>117.7</v>
       </c>
       <c r="J22" s="1">
-        <v>96.89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="5">
-        <v>29</v>
-      </c>
-      <c r="E23" s="8">
-        <v>183</v>
-      </c>
-      <c r="F23" s="8">
-        <v>80</v>
-      </c>
-      <c r="G23" s="3">
-        <v>23.888440980620498</v>
-      </c>
-      <c r="H23" s="1">
-        <v>117.7</v>
-      </c>
-      <c r="I23" s="1">
         <v>101.4</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K22" s="1">
         <v>80.97</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>